<commit_message>
version 1.5 added regex support
</commit_message>
<xml_diff>
--- a/convertextract/cors/correspondence_spreadsheets/heiltsuk_duolos.xlsx
+++ b/convertextract/cors/correspondence_spreadsheets/heiltsuk_duolos.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -348,7 +348,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -713,12 +713,12 @@
   <dimension ref="A1:B66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -726,7 +726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -734,15 +734,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -750,39 +750,39 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -790,15 +790,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -806,39 +806,39 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -846,7 +846,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -854,15 +854,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -870,47 +870,47 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" t="s">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" t="s">
         <v>100</v>
       </c>
-      <c r="B24" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -918,39 +918,39 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" t="s">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" t="s">
         <v>24</v>
       </c>
-      <c r="B27" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" t="s">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" t="s">
         <v>27</v>
       </c>
-      <c r="B29" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -958,7 +958,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -966,15 +966,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" t="s">
         <v>30</v>
       </c>
-      <c r="B32" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -982,7 +982,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -990,31 +990,31 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" t="s">
         <v>33</v>
       </c>
-      <c r="B35" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" t="s">
         <v>34</v>
       </c>
-      <c r="B36" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" t="s">
         <v>35</v>
       </c>
-      <c r="B37" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1030,15 +1030,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" t="s">
         <v>38</v>
       </c>
-      <c r="B40" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1054,15 +1054,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>94</v>
+      </c>
+      <c r="B43" t="s">
         <v>41</v>
       </c>
-      <c r="B43" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>85</v>
       </c>
@@ -1070,31 +1070,31 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>72</v>
+      </c>
+      <c r="B45" t="s">
         <v>42</v>
       </c>
-      <c r="B45" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" t="s">
         <v>43</v>
       </c>
-      <c r="B46" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>86</v>
+      </c>
+      <c r="B47" t="s">
         <v>44</v>
       </c>
-      <c r="B47" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -1102,31 +1102,31 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>90</v>
+      </c>
+      <c r="B49" t="s">
         <v>46</v>
       </c>
-      <c r="B49" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" t="s">
         <v>47</v>
       </c>
-      <c r="B50" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51" t="s">
         <v>48</v>
       </c>
-      <c r="B51" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -1134,23 +1134,23 @@
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53" t="s">
         <v>50</v>
       </c>
-      <c r="B53" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>64</v>
+      </c>
+      <c r="B54" t="s">
         <v>51</v>
       </c>
-      <c r="B54" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -1158,15 +1158,15 @@
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56" t="s">
         <v>53</v>
       </c>
-      <c r="B56" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>54</v>
       </c>
@@ -1174,76 +1174,76 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" t="s">
         <v>55</v>
       </c>
-      <c r="B58" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
+        <v>89</v>
+      </c>
+      <c r="B59" t="s">
         <v>56</v>
       </c>
-      <c r="B59" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>81</v>
+      </c>
+      <c r="B60" t="s">
         <v>57</v>
       </c>
-      <c r="B60" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>67</v>
+      </c>
+      <c r="B61" t="s">
         <v>58</v>
       </c>
-      <c r="B61" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A62" s="1" t="s">
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>98</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B62" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
+    </row>
+    <row r="63" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B63" t="s">
         <v>102</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
+        <v>103</v>
+      </c>
+      <c r="B64" t="s">
         <v>104</v>
       </c>
-      <c r="B64" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
+        <v>105</v>
+      </c>
+      <c r="B65" t="s">
         <v>104</v>
       </c>
-      <c r="B65" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
+        <v>106</v>
+      </c>
+      <c r="B66" t="s">
         <v>107</v>
-      </c>
-      <c r="B66" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>